<commit_message>
se agrega codigo donde permite estar el metodo close en un libro no abierto
</commit_message>
<xml_diff>
--- a/Formato de pagos/Bancolombia/Bancolombia 10-11-2020.xlsx
+++ b/Formato de pagos/Bancolombia/Bancolombia 10-11-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Diana\Formato de pagos\Bancolombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CCDB41-A405-4FDE-8EEE-F7FD1500D7C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DB11B5-B133-4EB8-86BF-E78BE8B00B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B485723B-909D-4E14-8ED0-E7823B8AF014}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D478B287-C80C-4833-83F1-D87644573968}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t xml:space="preserve"> Tipo de Identificacion</t>
   </si>
@@ -59,19 +59,82 @@
     <t>valor del pago</t>
   </si>
   <si>
+    <t>BIBO SOLUTIONS</t>
+  </si>
+  <si>
+    <t>SAS</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>83645289326</t>
+  </si>
+  <si>
+    <t>CIMAZ S.A.S</t>
+  </si>
+  <si>
+    <t>CIMPRE</t>
+  </si>
+  <si>
+    <t>SALUD OCUPACIONAL S.A.S.</t>
+  </si>
+  <si>
+    <t>IMPATA RESTREPO DIANA CARINA</t>
+  </si>
+  <si>
+    <t>DIGITALTIC SAS</t>
+  </si>
+  <si>
     <t>DOMINGO IGNACIO</t>
   </si>
   <si>
     <t>ROJAS</t>
   </si>
   <si>
-    <t>CA</t>
-  </si>
-  <si>
     <t>24003323467</t>
   </si>
   <si>
+    <t>ELECTRICOS DEL VALLE SA</t>
+  </si>
+  <si>
+    <t>ELECTRO JAPONESA S.A.</t>
+  </si>
+  <si>
+    <t>GVS COLOMBIA SAS</t>
+  </si>
+  <si>
     <t>Hp Financial Services Colombia LLC Sucursal Colombia</t>
+  </si>
+  <si>
+    <t>IZC</t>
+  </si>
+  <si>
+    <t>MAYORISTA SAS</t>
+  </si>
+  <si>
+    <t>JUAN CARLOS</t>
+  </si>
+  <si>
+    <t>MARQUEZ SANCHEZ</t>
+  </si>
+  <si>
+    <t>03165339508</t>
+  </si>
+  <si>
+    <t>LILIUM TECNOLOGIA SAS</t>
+  </si>
+  <si>
+    <t>NEXSYS DE COLOMBIA SA</t>
+  </si>
+  <si>
+    <t>RENTEK SAS</t>
+  </si>
+  <si>
+    <t>TIENDAS TECNOPLAZA S.A.S</t>
+  </si>
+  <si>
+    <t>ROJAS SALAZAR WILLIAM</t>
   </si>
   <si>
     <t>YAMAKI SAS</t>
@@ -450,9 +513,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DFE2FC-AA13-4012-9E4A-98C6E4E6D47A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFA4E579-08CD-45BA-92C4-2B9F8E3107AA}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -463,7 +526,7 @@
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
@@ -498,10 +561,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>7215649</v>
+        <v>900858550</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -510,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="1">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>10</v>
@@ -519,7 +582,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="1">
-        <v>97991</v>
+        <v>2359386</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -527,13 +590,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>830076882</v>
+        <v>900654100</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H3" s="1">
-        <v>4407849</v>
+        <v>525870</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -541,12 +604,252 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>800179308</v>
+        <v>1143940723</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H4" s="1">
+        <v>87451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>31322510</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>84300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>901223156</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="1">
+        <v>193970</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7215649</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1">
+        <v>97991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>890304345</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1">
+        <v>172500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>890306372</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1819546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>900298074</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1">
+        <v>9952604</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>830076882</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1">
+        <v>4407849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1143940722</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1">
+        <v>52092009</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1">
+        <v>94281756</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1074121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>900892841</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H14" s="1">
+        <v>669600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>800035776</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1">
+        <v>18089916</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="1">
+        <v>830034343</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="1">
+        <v>4094318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>900355222</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="1">
+        <v>492503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7685100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="1">
+        <v>6013778</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1">
+        <v>800179308</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="1">
         <v>4031339</v>
       </c>
     </row>

</xml_diff>